<commit_message>
name changed and added support for os path
</commit_message>
<xml_diff>
--- a/Daily timesheet.xlsx
+++ b/Daily timesheet.xlsx
@@ -334,7 +334,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -674,6 +674,50 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>02/03/2023</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>meeting internally on to discuss on EIR implementation plan</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>02/03/2023</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>wrote a reply letter on DHIS2 user accounts leakage notified by department of cyber security</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -685,7 +729,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -831,6 +875,72 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>02/03/2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>meeting on pre-bid closing</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>05/03/2023</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>prepared presentation for bid closing to the committee</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>dne</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>05/03/2023</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>meeting with bid committee to finalize winning bidder of eBRS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2.5</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>done</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>